<commit_message>
Just changed few column headings
</commit_message>
<xml_diff>
--- a/Dispersion rate calculation.xlsx
+++ b/Dispersion rate calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_31f7\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashif\OneDrive - Airzai\Airzai\GitHub\Airzai-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{2F4D0091-19E2-48A9-9B81-03C860113F85}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{7CC2387D-AE91-48C3-8199-F0F9B88BF952}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Unit No.#</t>
   </si>
@@ -57,25 +57,34 @@
     <t>Test unit 08</t>
   </si>
   <si>
-    <t>Total fragrance dispersed</t>
-  </si>
-  <si>
     <t>Test unit 10</t>
   </si>
   <si>
-    <t xml:space="preserve">Average </t>
-  </si>
-  <si>
     <t>Test unit 07</t>
   </si>
   <si>
     <t>Rosepetale</t>
   </si>
   <si>
-    <t>No. of Bursts/hr</t>
-  </si>
-  <si>
     <t>Initial Cartridge level (ml)</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Augus 7th - 12th</t>
+  </si>
+  <si>
+    <t>Total fragrance dispersed (ml)</t>
+  </si>
+  <si>
+    <t>Total ON time per Hr</t>
+  </si>
+  <si>
+    <t>400 Sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensual musk Average </t>
   </si>
 </sst>
 </file>
@@ -99,12 +108,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,9 +134,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,196 +463,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="6" width="30.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="1" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="7" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>27.5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="F4" s="3">
+        <v>50</v>
+      </c>
+      <c r="G4" s="3">
+        <f>(F4-E4)</f>
+        <v>38.5</v>
+      </c>
+      <c r="H4" s="3">
+        <f>(G4/C4)</f>
+        <v>1.4</v>
+      </c>
+      <c r="I4" s="3">
+        <f>(H4/3600)</f>
+        <v>3.8888888888888887E-4</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3">
+        <f>(F5-E5)</f>
+        <v>44.5</v>
+      </c>
+      <c r="H5" s="3">
+        <f>(G5/C5)</f>
+        <v>1.3692307692307693</v>
+      </c>
+      <c r="I5" s="3">
+        <f>(H5/3600)</f>
+        <v>3.8034188034188036E-4</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="3">
+        <v>20.5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>50</v>
+      </c>
+      <c r="G6" s="3">
+        <f>(F6-E6)</f>
+        <v>25</v>
+      </c>
+      <c r="H6" s="3">
+        <f>(G6/C6)</f>
+        <v>1.2195121951219512</v>
+      </c>
+      <c r="I6" s="3">
+        <f>(H6/3600)</f>
+        <v>3.3875338753387534E-4</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>27.5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>11.5</v>
-      </c>
-      <c r="E4">
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="4">
+        <f>AVERAGE(H4:H8)</f>
+        <v>1.3295809881175735</v>
+      </c>
+      <c r="I9" s="4">
+        <f>AVERAGE(I4:I8)</f>
+        <v>3.693280522548815E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3">
+        <v>20.5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3">
         <v>50</v>
       </c>
-      <c r="F4">
-        <f>(E4-D4)</f>
-        <v>38.5</v>
-      </c>
-      <c r="G4">
-        <f>(F4/B4)</f>
-        <v>1.4</v>
-      </c>
-      <c r="H4">
-        <f>(G4/3600)</f>
-        <v>3.8888888888888887E-4</v>
-      </c>
-      <c r="I4">
-        <v>80</v>
+      <c r="G12" s="3">
+        <f>(F12-E12)</f>
+        <v>40</v>
+      </c>
+      <c r="H12" s="3">
+        <f>(G12/C12)</f>
+        <v>1.9512195121951219</v>
+      </c>
+      <c r="I12" s="3">
+        <f>(H12/3600)</f>
+        <v>5.4200542005420054E-4</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>32.5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>5.5</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <f>(E5-D5)</f>
-        <v>44.5</v>
-      </c>
-      <c r="G5">
-        <f>(F5/B5)</f>
-        <v>1.3692307692307693</v>
-      </c>
-      <c r="H5">
-        <f>(G5/3600)</f>
-        <v>3.8034188034188036E-4</v>
-      </c>
-      <c r="I5">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>20.5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>25</v>
-      </c>
-      <c r="E6">
-        <v>50</v>
-      </c>
-      <c r="F6">
-        <f>(E6-D6)</f>
-        <v>25</v>
-      </c>
-      <c r="G6">
-        <f>(F6/B6)</f>
-        <v>1.2195121951219512</v>
-      </c>
-      <c r="H6">
-        <f>(G6/3600)</f>
-        <v>3.3875338753387534E-4</v>
-      </c>
-      <c r="I6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="1">
-        <f>AVERAGE(G4:G8)</f>
-        <v>1.3295809881175735</v>
-      </c>
-      <c r="H9" s="1">
-        <f>AVERAGE(H4:H8)</f>
-        <v>3.693280522548815E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>20.5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>50</v>
-      </c>
-      <c r="F12">
-        <f>(E12-D12)</f>
-        <v>40</v>
-      </c>
-      <c r="G12">
-        <f>(F12/B12)</f>
-        <v>1.9512195121951219</v>
-      </c>
-      <c r="H12">
-        <f>(G12/3600)</f>
-        <v>5.4200542005420054E-4</v>
-      </c>
-      <c r="I12">
-        <v>80</v>
-      </c>
-    </row>
+    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Rosepetale results
</commit_message>
<xml_diff>
--- a/Dispersion rate calculation.xlsx
+++ b/Dispersion rate calculation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashif\OneDrive - Airzai\Airzai\GitHub\Airzai-Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajeeth\OneDrive\Weekly updates\GitHub\Airzai-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{7CC2387D-AE91-48C3-8199-F0F9B88BF952}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{CACA060C-1A4E-4737-A786-91D76C1C99D4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Unit No.#</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Augus 7th - 12th</t>
-  </si>
-  <si>
     <t>Total fragrance dispersed (ml)</t>
   </si>
   <si>
@@ -85,6 +82,15 @@
   </si>
   <si>
     <t xml:space="preserve">Sensual musk Average </t>
+  </si>
+  <si>
+    <t>Test unit 06</t>
+  </si>
+  <si>
+    <t>August 12th-14th</t>
+  </si>
+  <si>
+    <t>August 7th - 12th</t>
   </si>
 </sst>
 </file>
@@ -466,7 +472,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +509,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
@@ -512,7 +518,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -521,7 +527,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
         <v>27.5</v>
@@ -548,7 +554,7 @@
         <v>3.8888888888888887E-4</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -556,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
         <v>32.5</v>
@@ -583,7 +589,7 @@
         <v>3.8034188034188036E-4</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -591,7 +597,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
         <v>20.5</v>
@@ -618,14 +624,14 @@
         <v>3.3875338753387534E-4</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="4">
         <f>AVERAGE(H4:H8)</f>
@@ -640,37 +646,74 @@
     <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C12" s="3">
-        <v>20.5</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F12" s="3">
         <v>50</v>
       </c>
       <c r="G12" s="3">
         <f>(F12-E12)</f>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H12" s="3">
         <f>(G12/C12)</f>
-        <v>1.9512195121951219</v>
+        <v>1.875</v>
       </c>
       <c r="I12" s="3">
         <f>(H12/3600)</f>
-        <v>5.4200542005420054E-4</v>
+        <v>5.2083333333333333E-4</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3">
+        <v>20.5</v>
+      </c>
+      <c r="F13" s="3">
+        <v>50</v>
+      </c>
+      <c r="G13" s="3">
+        <f>(F13-E13)</f>
+        <v>29.5</v>
+      </c>
+      <c r="H13" s="3">
+        <f>(G13/C13)</f>
+        <v>1.84375</v>
+      </c>
+      <c r="I13" s="3">
+        <f>(H13/3600)</f>
+        <v>5.1215277777777782E-4</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
synthetic wick dispersion rate updated
</commit_message>
<xml_diff>
--- a/Dispersion rate calculation.xlsx
+++ b/Dispersion rate calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajeeth\OneDrive\Weekly updates\GitHub\Airzai-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{CACA060C-1A4E-4737-A786-91D76C1C99D4}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{F95EAFC1-A9D0-4C15-A876-0097238358B7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Unit No.#</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>August 7th - 12th</t>
+  </si>
+  <si>
+    <t>August 14th</t>
+  </si>
+  <si>
+    <t>Test unit 08 (Synthetic wick)</t>
   </si>
 </sst>
 </file>
@@ -472,12 +478,13 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="4" width="27.7109375" customWidth="1"/>
     <col min="5" max="7" width="30.85546875" customWidth="1"/>
     <col min="8" max="8" width="29.28515625" customWidth="1"/>
@@ -714,7 +721,41 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3">
+        <v>42</v>
+      </c>
+      <c r="F14" s="3">
+        <v>50</v>
+      </c>
+      <c r="G14" s="3">
+        <f>(F14-E14)</f>
+        <v>8</v>
+      </c>
+      <c r="H14" s="3">
+        <f>(G14/C14)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I14" s="3">
+        <f>(H14/3600)</f>
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Dispersion rate calculation.xlsx
</commit_message>
<xml_diff>
--- a/Dispersion rate calculation.xlsx
+++ b/Dispersion rate calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajeeth\OneDrive\Weekly updates\GitHub\Airzai-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{F95EAFC1-A9D0-4C15-A876-0097238358B7}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{44394EE9-3ED7-45FA-93D0-29E4C42E22EF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>